<commit_message>
Remove duplicate caseworker-caa event authorisations
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_Duplicate_Priority.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_Duplicate_Priority.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Desktop/RDM-9555/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellysiak/development/ccd/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A361BF5C-B357-194D-8EC9-5E4576C67446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8485DA35-58A7-3E45-B945-3278C13F0099}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="33600" windowHeight="19340" firstSheet="14" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5926" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5922" uniqueCount="980">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -12684,7 +12684,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F50" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F49" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
@@ -17777,7 +17777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D5" zoomScale="109" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D5" zoomScale="109" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -33922,10 +33922,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:EK50"/>
+  <dimension ref="A1:EK49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -33938,7 +33938,7 @@
     <col min="7" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:141" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="198" t="s">
         <v>702</v>
       </c>
@@ -33954,7 +33954,7 @@
       <c r="E1" s="81"/>
       <c r="F1" s="81"/>
     </row>
-    <row r="2" spans="1:6" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:141" ht="65" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="163" t="s">
         <v>4</v>
       </c>
@@ -33974,7 +33974,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="57" t="s">
         <v>9</v>
       </c>
@@ -33994,7 +33994,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="60">
         <v>42736</v>
       </c>
@@ -34012,7 +34012,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="60">
         <v>42736</v>
       </c>
@@ -34030,7 +34030,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="60">
         <v>42736</v>
       </c>
@@ -34048,7 +34048,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="60">
         <v>42736</v>
       </c>
@@ -34066,25 +34066,25 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="60">
         <v>42736</v>
       </c>
       <c r="B8" s="81"/>
       <c r="C8" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>941</v>
+        <v>880</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>392</v>
       </c>
       <c r="E8" s="134" t="s">
-        <v>936</v>
+        <v>776</v>
       </c>
       <c r="F8" s="115" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="60">
         <v>42736</v>
       </c>
@@ -34092,8 +34092,8 @@
       <c r="C9" s="62" t="s">
         <v>880</v>
       </c>
-      <c r="D9" s="62" t="s">
-        <v>392</v>
+      <c r="D9" s="65" t="s">
+        <v>535</v>
       </c>
       <c r="E9" s="134" t="s">
         <v>776</v>
@@ -34102,16 +34102,16 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="60">
         <v>42736</v>
       </c>
       <c r="B10" s="81"/>
-      <c r="C10" s="62" t="s">
-        <v>880</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>535</v>
+      <c r="C10" s="65" t="s">
+        <v>881</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>392</v>
       </c>
       <c r="E10" s="134" t="s">
         <v>776</v>
@@ -34120,43 +34120,43 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="65" t="s">
+    <row r="11" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="84"/>
+      <c r="C11" s="118" t="s">
         <v>881</v>
       </c>
-      <c r="D11" s="62" t="s">
-        <v>392</v>
+      <c r="D11" s="118" t="s">
+        <v>388</v>
       </c>
       <c r="E11" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F11" s="115" t="s">
+      <c r="F11" s="119" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="118" t="s">
+    <row r="12" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="81"/>
+      <c r="C12" s="120" t="s">
         <v>881</v>
       </c>
-      <c r="D12" s="118" t="s">
-        <v>388</v>
+      <c r="D12" s="120" t="s">
+        <v>373</v>
       </c>
       <c r="E12" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F12" s="119" t="s">
+      <c r="F12" s="115" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="60">
         <v>42736</v>
       </c>
@@ -34165,7 +34165,7 @@
         <v>881</v>
       </c>
       <c r="D13" s="120" t="s">
-        <v>373</v>
+        <v>542</v>
       </c>
       <c r="E13" s="134" t="s">
         <v>776</v>
@@ -34174,7 +34174,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="60">
         <v>42736</v>
       </c>
@@ -34183,7 +34183,7 @@
         <v>881</v>
       </c>
       <c r="D14" s="120" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E14" s="134" t="s">
         <v>776</v>
@@ -34192,57 +34192,192 @@
         <v>339</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B15" s="81"/>
+    <row r="15" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B15" s="84"/>
       <c r="C15" s="120" t="s">
         <v>881</v>
       </c>
       <c r="D15" s="120" t="s">
-        <v>544</v>
+        <v>953</v>
       </c>
       <c r="E15" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F15" s="115" t="s">
+      <c r="F15" s="119" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="120" t="s">
-        <v>881</v>
-      </c>
-      <c r="D16" s="120" t="s">
-        <v>953</v>
-      </c>
-      <c r="E16" s="134" t="s">
+    <row r="16" spans="1:141" s="292" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="344">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="337"/>
+      <c r="C16" s="293" t="s">
+        <v>922</v>
+      </c>
+      <c r="D16" s="293" t="s">
+        <v>924</v>
+      </c>
+      <c r="E16" s="366" t="s">
         <v>776</v>
       </c>
-      <c r="F16" s="119" t="s">
+      <c r="F16" s="362" t="s">
         <v>339</v>
       </c>
+      <c r="G16" s="400"/>
+      <c r="H16" s="400"/>
+      <c r="I16" s="400"/>
+      <c r="J16" s="400"/>
+      <c r="K16" s="400"/>
+      <c r="L16" s="400"/>
+      <c r="M16" s="400"/>
+      <c r="N16" s="400"/>
+      <c r="O16" s="400"/>
+      <c r="P16" s="400"/>
+      <c r="Q16" s="400"/>
+      <c r="R16" s="400"/>
+      <c r="S16" s="400"/>
+      <c r="T16" s="400"/>
+      <c r="U16" s="400"/>
+      <c r="V16" s="400"/>
+      <c r="W16" s="400"/>
+      <c r="X16" s="400"/>
+      <c r="Y16" s="400"/>
+      <c r="Z16" s="400"/>
+      <c r="AA16" s="400"/>
+      <c r="AB16" s="400"/>
+      <c r="AC16" s="400"/>
+      <c r="AD16" s="400"/>
+      <c r="AE16" s="400"/>
+      <c r="AF16" s="400"/>
+      <c r="AG16" s="400"/>
+      <c r="AH16" s="400"/>
+      <c r="AI16" s="400"/>
+      <c r="AJ16" s="400"/>
+      <c r="AK16" s="400"/>
+      <c r="AL16" s="400"/>
+      <c r="AM16" s="400"/>
+      <c r="AN16" s="400"/>
+      <c r="AO16" s="400"/>
+      <c r="AP16" s="400"/>
+      <c r="AQ16" s="400"/>
+      <c r="AR16" s="400"/>
+      <c r="AS16" s="400"/>
+      <c r="AT16" s="400"/>
+      <c r="AU16" s="400"/>
+      <c r="AV16" s="400"/>
+      <c r="AW16" s="400"/>
+      <c r="AX16" s="400"/>
+      <c r="AY16" s="400"/>
+      <c r="AZ16" s="400"/>
+      <c r="BA16" s="400"/>
+      <c r="BB16" s="400"/>
+      <c r="BC16" s="400"/>
+      <c r="BD16" s="400"/>
+      <c r="BE16" s="400"/>
+      <c r="BF16" s="400"/>
+      <c r="BG16" s="400"/>
+      <c r="BH16" s="400"/>
+      <c r="BI16" s="400"/>
+      <c r="BJ16" s="400"/>
+      <c r="BK16" s="400"/>
+      <c r="BL16" s="400"/>
+      <c r="BM16" s="400"/>
+      <c r="BN16" s="400"/>
+      <c r="BO16" s="400"/>
+      <c r="BP16" s="400"/>
+      <c r="BQ16" s="400"/>
+      <c r="BR16" s="400"/>
+      <c r="BS16" s="400"/>
+      <c r="BT16" s="400"/>
+      <c r="BU16" s="400"/>
+      <c r="BV16" s="400"/>
+      <c r="BW16" s="400"/>
+      <c r="BX16" s="400"/>
+      <c r="BY16" s="400"/>
+      <c r="BZ16" s="400"/>
+      <c r="CA16" s="400"/>
+      <c r="CB16" s="400"/>
+      <c r="CC16" s="400"/>
+      <c r="CD16" s="400"/>
+      <c r="CE16" s="400"/>
+      <c r="CF16" s="400"/>
+      <c r="CG16" s="400"/>
+      <c r="CH16" s="400"/>
+      <c r="CI16" s="400"/>
+      <c r="CJ16" s="400"/>
+      <c r="CK16" s="400"/>
+      <c r="CL16" s="400"/>
+      <c r="CM16" s="400"/>
+      <c r="CN16" s="400"/>
+      <c r="CO16" s="400"/>
+      <c r="CP16" s="400"/>
+      <c r="CQ16" s="400"/>
+      <c r="CR16" s="400"/>
+      <c r="CS16" s="400"/>
+      <c r="CT16" s="400"/>
+      <c r="CU16" s="400"/>
+      <c r="CV16" s="400"/>
+      <c r="CW16" s="400"/>
+      <c r="CX16" s="400"/>
+      <c r="CY16" s="400"/>
+      <c r="CZ16" s="400"/>
+      <c r="DA16" s="400"/>
+      <c r="DB16" s="400"/>
+      <c r="DC16" s="400"/>
+      <c r="DD16" s="400"/>
+      <c r="DE16" s="400"/>
+      <c r="DF16" s="400"/>
+      <c r="DG16" s="400"/>
+      <c r="DH16" s="400"/>
+      <c r="DI16" s="400"/>
+      <c r="DJ16" s="400"/>
+      <c r="DK16" s="400"/>
+      <c r="DL16" s="400"/>
+      <c r="DM16" s="400"/>
+      <c r="DN16" s="400"/>
+      <c r="DO16" s="400"/>
+      <c r="DP16" s="400"/>
+      <c r="DQ16" s="400"/>
+      <c r="DR16" s="400"/>
+      <c r="DS16" s="400"/>
+      <c r="DT16" s="400"/>
+      <c r="DU16" s="400"/>
+      <c r="DV16" s="400"/>
+      <c r="DW16" s="400"/>
+      <c r="DX16" s="400"/>
+      <c r="DY16" s="400"/>
+      <c r="DZ16" s="400"/>
+      <c r="EA16" s="400"/>
+      <c r="EB16" s="400"/>
+      <c r="EC16" s="400"/>
+      <c r="ED16" s="400"/>
+      <c r="EE16" s="400"/>
+      <c r="EF16" s="400"/>
+      <c r="EG16" s="400"/>
+      <c r="EH16" s="400"/>
+      <c r="EI16" s="400"/>
+      <c r="EJ16" s="400"/>
+      <c r="EK16" s="400"/>
     </row>
     <row r="17" spans="1:141" s="292" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="344">
-        <v>42736</v>
-      </c>
-      <c r="B17" s="337"/>
+      <c r="A17" s="286">
+        <v>42736</v>
+      </c>
+      <c r="B17" s="289"/>
       <c r="C17" s="293" t="s">
         <v>922</v>
       </c>
       <c r="D17" s="293" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E17" s="366" t="s">
         <v>776</v>
       </c>
-      <c r="F17" s="362" t="s">
+      <c r="F17" s="294" t="s">
         <v>339</v>
       </c>
       <c r="G17" s="400"/>
@@ -34381,158 +34516,23 @@
       <c r="EJ17" s="400"/>
       <c r="EK17" s="400"/>
     </row>
-    <row r="18" spans="1:141" s="292" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="286">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="289"/>
-      <c r="C18" s="293" t="s">
-        <v>922</v>
-      </c>
-      <c r="D18" s="293" t="s">
-        <v>923</v>
-      </c>
-      <c r="E18" s="366" t="s">
+    <row r="18" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="81"/>
+      <c r="C18" s="65" t="s">
+        <v>883</v>
+      </c>
+      <c r="D18" s="62" t="s">
+        <v>392</v>
+      </c>
+      <c r="E18" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F18" s="294" t="s">
+      <c r="F18" s="115" t="s">
         <v>339</v>
       </c>
-      <c r="G18" s="400"/>
-      <c r="H18" s="400"/>
-      <c r="I18" s="400"/>
-      <c r="J18" s="400"/>
-      <c r="K18" s="400"/>
-      <c r="L18" s="400"/>
-      <c r="M18" s="400"/>
-      <c r="N18" s="400"/>
-      <c r="O18" s="400"/>
-      <c r="P18" s="400"/>
-      <c r="Q18" s="400"/>
-      <c r="R18" s="400"/>
-      <c r="S18" s="400"/>
-      <c r="T18" s="400"/>
-      <c r="U18" s="400"/>
-      <c r="V18" s="400"/>
-      <c r="W18" s="400"/>
-      <c r="X18" s="400"/>
-      <c r="Y18" s="400"/>
-      <c r="Z18" s="400"/>
-      <c r="AA18" s="400"/>
-      <c r="AB18" s="400"/>
-      <c r="AC18" s="400"/>
-      <c r="AD18" s="400"/>
-      <c r="AE18" s="400"/>
-      <c r="AF18" s="400"/>
-      <c r="AG18" s="400"/>
-      <c r="AH18" s="400"/>
-      <c r="AI18" s="400"/>
-      <c r="AJ18" s="400"/>
-      <c r="AK18" s="400"/>
-      <c r="AL18" s="400"/>
-      <c r="AM18" s="400"/>
-      <c r="AN18" s="400"/>
-      <c r="AO18" s="400"/>
-      <c r="AP18" s="400"/>
-      <c r="AQ18" s="400"/>
-      <c r="AR18" s="400"/>
-      <c r="AS18" s="400"/>
-      <c r="AT18" s="400"/>
-      <c r="AU18" s="400"/>
-      <c r="AV18" s="400"/>
-      <c r="AW18" s="400"/>
-      <c r="AX18" s="400"/>
-      <c r="AY18" s="400"/>
-      <c r="AZ18" s="400"/>
-      <c r="BA18" s="400"/>
-      <c r="BB18" s="400"/>
-      <c r="BC18" s="400"/>
-      <c r="BD18" s="400"/>
-      <c r="BE18" s="400"/>
-      <c r="BF18" s="400"/>
-      <c r="BG18" s="400"/>
-      <c r="BH18" s="400"/>
-      <c r="BI18" s="400"/>
-      <c r="BJ18" s="400"/>
-      <c r="BK18" s="400"/>
-      <c r="BL18" s="400"/>
-      <c r="BM18" s="400"/>
-      <c r="BN18" s="400"/>
-      <c r="BO18" s="400"/>
-      <c r="BP18" s="400"/>
-      <c r="BQ18" s="400"/>
-      <c r="BR18" s="400"/>
-      <c r="BS18" s="400"/>
-      <c r="BT18" s="400"/>
-      <c r="BU18" s="400"/>
-      <c r="BV18" s="400"/>
-      <c r="BW18" s="400"/>
-      <c r="BX18" s="400"/>
-      <c r="BY18" s="400"/>
-      <c r="BZ18" s="400"/>
-      <c r="CA18" s="400"/>
-      <c r="CB18" s="400"/>
-      <c r="CC18" s="400"/>
-      <c r="CD18" s="400"/>
-      <c r="CE18" s="400"/>
-      <c r="CF18" s="400"/>
-      <c r="CG18" s="400"/>
-      <c r="CH18" s="400"/>
-      <c r="CI18" s="400"/>
-      <c r="CJ18" s="400"/>
-      <c r="CK18" s="400"/>
-      <c r="CL18" s="400"/>
-      <c r="CM18" s="400"/>
-      <c r="CN18" s="400"/>
-      <c r="CO18" s="400"/>
-      <c r="CP18" s="400"/>
-      <c r="CQ18" s="400"/>
-      <c r="CR18" s="400"/>
-      <c r="CS18" s="400"/>
-      <c r="CT18" s="400"/>
-      <c r="CU18" s="400"/>
-      <c r="CV18" s="400"/>
-      <c r="CW18" s="400"/>
-      <c r="CX18" s="400"/>
-      <c r="CY18" s="400"/>
-      <c r="CZ18" s="400"/>
-      <c r="DA18" s="400"/>
-      <c r="DB18" s="400"/>
-      <c r="DC18" s="400"/>
-      <c r="DD18" s="400"/>
-      <c r="DE18" s="400"/>
-      <c r="DF18" s="400"/>
-      <c r="DG18" s="400"/>
-      <c r="DH18" s="400"/>
-      <c r="DI18" s="400"/>
-      <c r="DJ18" s="400"/>
-      <c r="DK18" s="400"/>
-      <c r="DL18" s="400"/>
-      <c r="DM18" s="400"/>
-      <c r="DN18" s="400"/>
-      <c r="DO18" s="400"/>
-      <c r="DP18" s="400"/>
-      <c r="DQ18" s="400"/>
-      <c r="DR18" s="400"/>
-      <c r="DS18" s="400"/>
-      <c r="DT18" s="400"/>
-      <c r="DU18" s="400"/>
-      <c r="DV18" s="400"/>
-      <c r="DW18" s="400"/>
-      <c r="DX18" s="400"/>
-      <c r="DY18" s="400"/>
-      <c r="DZ18" s="400"/>
-      <c r="EA18" s="400"/>
-      <c r="EB18" s="400"/>
-      <c r="EC18" s="400"/>
-      <c r="ED18" s="400"/>
-      <c r="EE18" s="400"/>
-      <c r="EF18" s="400"/>
-      <c r="EG18" s="400"/>
-      <c r="EH18" s="400"/>
-      <c r="EI18" s="400"/>
-      <c r="EJ18" s="400"/>
-      <c r="EK18" s="400"/>
     </row>
     <row r="19" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="60">
@@ -34540,7 +34540,7 @@
       </c>
       <c r="B19" s="81"/>
       <c r="C19" s="65" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="D19" s="62" t="s">
         <v>392</v>
@@ -34561,7 +34561,7 @@
         <v>884</v>
       </c>
       <c r="D20" s="62" t="s">
-        <v>392</v>
+        <v>546</v>
       </c>
       <c r="E20" s="134" t="s">
         <v>776</v>
@@ -34579,7 +34579,7 @@
         <v>884</v>
       </c>
       <c r="D21" s="62" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E21" s="134" t="s">
         <v>776</v>
@@ -34597,7 +34597,7 @@
         <v>884</v>
       </c>
       <c r="D22" s="62" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E22" s="134" t="s">
         <v>776</v>
@@ -34615,7 +34615,7 @@
         <v>884</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="E23" s="134" t="s">
         <v>776</v>
@@ -34624,16 +34624,16 @@
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="60">
         <v>42736</v>
       </c>
       <c r="B24" s="81"/>
-      <c r="C24" s="65" t="s">
-        <v>884</v>
+      <c r="C24" s="62" t="s">
+        <v>885</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>552</v>
+        <v>392</v>
       </c>
       <c r="E24" s="134" t="s">
         <v>776</v>
@@ -34642,13 +34642,13 @@
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="60">
         <v>42736</v>
       </c>
       <c r="B25" s="81"/>
       <c r="C25" s="62" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="D25" s="62" t="s">
         <v>392</v>
@@ -34661,20 +34661,20 @@
       </c>
     </row>
     <row r="26" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B26" s="81"/>
-      <c r="C26" s="62" t="s">
+      <c r="A26" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B26" s="84"/>
+      <c r="C26" s="68" t="s">
         <v>886</v>
       </c>
-      <c r="D26" s="62" t="s">
-        <v>392</v>
+      <c r="D26" s="68" t="s">
+        <v>555</v>
       </c>
       <c r="E26" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F26" s="115" t="s">
+      <c r="F26" s="119" t="s">
         <v>339</v>
       </c>
     </row>
@@ -34687,7 +34687,7 @@
         <v>886</v>
       </c>
       <c r="D27" s="68" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="E27" s="134" t="s">
         <v>776</v>
@@ -34705,7 +34705,7 @@
         <v>886</v>
       </c>
       <c r="D28" s="68" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E28" s="134" t="s">
         <v>776</v>
@@ -34714,7 +34714,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="1:141" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="66">
         <v>42736</v>
       </c>
@@ -34723,7 +34723,7 @@
         <v>886</v>
       </c>
       <c r="D29" s="68" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="E29" s="134" t="s">
         <v>776</v>
@@ -34733,39 +34733,39 @@
       </c>
     </row>
     <row r="30" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B30" s="84"/>
-      <c r="C30" s="68" t="s">
-        <v>886</v>
-      </c>
-      <c r="D30" s="68" t="s">
-        <v>561</v>
+      <c r="A30" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="81"/>
+      <c r="C30" s="62" t="s">
+        <v>888</v>
+      </c>
+      <c r="D30" s="62" t="s">
+        <v>392</v>
       </c>
       <c r="E30" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F30" s="119" t="s">
-        <v>339</v>
+      <c r="F30" s="115" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B31" s="81"/>
-      <c r="C31" s="62" t="s">
-        <v>888</v>
-      </c>
-      <c r="D31" s="62" t="s">
+      <c r="A31" s="66">
+        <v>42736</v>
+      </c>
+      <c r="B31" s="84"/>
+      <c r="C31" s="84" t="s">
+        <v>887</v>
+      </c>
+      <c r="D31" s="65" t="s">
         <v>392</v>
       </c>
       <c r="E31" s="134" t="s">
         <v>776</v>
       </c>
-      <c r="F31" s="115" t="s">
-        <v>354</v>
+      <c r="F31" s="119" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:141" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -34776,8 +34776,8 @@
       <c r="C32" s="84" t="s">
         <v>887</v>
       </c>
-      <c r="D32" s="65" t="s">
-        <v>392</v>
+      <c r="D32" s="118" t="s">
+        <v>563</v>
       </c>
       <c r="E32" s="134" t="s">
         <v>776</v>
@@ -34795,7 +34795,7 @@
         <v>887</v>
       </c>
       <c r="D33" s="118" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="E33" s="134" t="s">
         <v>776</v>
@@ -34809,11 +34809,11 @@
         <v>42736</v>
       </c>
       <c r="B34" s="84"/>
-      <c r="C34" s="84" t="s">
-        <v>887</v>
-      </c>
-      <c r="D34" s="118" t="s">
-        <v>567</v>
+      <c r="C34" s="65" t="s">
+        <v>889</v>
+      </c>
+      <c r="D34" s="68" t="s">
+        <v>392</v>
       </c>
       <c r="E34" s="134" t="s">
         <v>776</v>
@@ -34827,14 +34827,14 @@
         <v>42736</v>
       </c>
       <c r="B35" s="84"/>
-      <c r="C35" s="65" t="s">
-        <v>889</v>
-      </c>
-      <c r="D35" s="68" t="s">
+      <c r="C35" s="68" t="s">
+        <v>892</v>
+      </c>
+      <c r="D35" s="82" t="s">
         <v>392</v>
       </c>
-      <c r="E35" s="134" t="s">
-        <v>776</v>
+      <c r="E35" s="84" t="s">
+        <v>777</v>
       </c>
       <c r="F35" s="119" t="s">
         <v>339</v>
@@ -34849,13 +34849,13 @@
         <v>892</v>
       </c>
       <c r="D36" s="82" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E36" s="84" t="s">
         <v>777</v>
       </c>
       <c r="F36" s="119" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -34867,13 +34867,13 @@
         <v>892</v>
       </c>
       <c r="D37" s="82" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E37" s="84" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F37" s="119" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -34885,16 +34885,16 @@
         <v>892</v>
       </c>
       <c r="D38" s="82" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E38" s="84" t="s">
         <v>778</v>
       </c>
       <c r="F38" s="119" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="66">
         <v>42736</v>
       </c>
@@ -34902,14 +34902,14 @@
       <c r="C39" s="68" t="s">
         <v>892</v>
       </c>
-      <c r="D39" s="82" t="s">
-        <v>393</v>
+      <c r="D39" s="68" t="s">
+        <v>394</v>
       </c>
       <c r="E39" s="84" t="s">
         <v>778</v>
       </c>
       <c r="F39" s="119" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -34924,7 +34924,7 @@
         <v>394</v>
       </c>
       <c r="E40" s="84" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F40" s="119" t="s">
         <v>340</v>
@@ -34935,20 +34935,20 @@
         <v>42736</v>
       </c>
       <c r="B41" s="84"/>
-      <c r="C41" s="68" t="s">
-        <v>892</v>
+      <c r="C41" s="65" t="s">
+        <v>890</v>
       </c>
       <c r="D41" s="68" t="s">
-        <v>394</v>
-      </c>
-      <c r="E41" s="84" t="s">
-        <v>777</v>
+        <v>392</v>
+      </c>
+      <c r="E41" s="134" t="s">
+        <v>776</v>
       </c>
       <c r="F41" s="119" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="66">
         <v>42736</v>
       </c>
@@ -34957,7 +34957,7 @@
         <v>890</v>
       </c>
       <c r="D42" s="68" t="s">
-        <v>392</v>
+        <v>729</v>
       </c>
       <c r="E42" s="134" t="s">
         <v>776</v>
@@ -34967,20 +34967,20 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="66">
-        <v>42736</v>
-      </c>
-      <c r="B43" s="84"/>
-      <c r="C43" s="65" t="s">
+      <c r="A43" s="71">
+        <v>42736</v>
+      </c>
+      <c r="B43" s="90"/>
+      <c r="C43" s="73" t="s">
         <v>890</v>
       </c>
-      <c r="D43" s="68" t="s">
-        <v>729</v>
-      </c>
-      <c r="E43" s="134" t="s">
+      <c r="D43" s="86" t="s">
+        <v>732</v>
+      </c>
+      <c r="E43" s="195" t="s">
         <v>776</v>
       </c>
-      <c r="F43" s="119" t="s">
+      <c r="F43" s="125" t="s">
         <v>339</v>
       </c>
     </row>
@@ -34988,12 +34988,12 @@
       <c r="A44" s="71">
         <v>42736</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="73" t="s">
-        <v>890</v>
-      </c>
-      <c r="D44" s="86" t="s">
-        <v>732</v>
+      <c r="B44" s="69"/>
+      <c r="C44" s="65" t="s">
+        <v>891</v>
+      </c>
+      <c r="D44" s="82" t="s">
+        <v>834</v>
       </c>
       <c r="E44" s="195" t="s">
         <v>776</v>
@@ -35011,7 +35011,7 @@
         <v>891</v>
       </c>
       <c r="D45" s="82" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="E45" s="195" t="s">
         <v>776</v>
@@ -35029,7 +35029,7 @@
         <v>891</v>
       </c>
       <c r="D46" s="82" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="E46" s="195" t="s">
         <v>776</v>
@@ -35042,12 +35042,12 @@
       <c r="A47" s="71">
         <v>42736</v>
       </c>
-      <c r="B47" s="69"/>
+      <c r="B47" s="72"/>
       <c r="C47" s="65" t="s">
         <v>891</v>
       </c>
-      <c r="D47" s="82" t="s">
-        <v>839</v>
+      <c r="D47" s="88" t="s">
+        <v>841</v>
       </c>
       <c r="E47" s="195" t="s">
         <v>776</v>
@@ -35057,56 +35057,38 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="71">
-        <v>42736</v>
-      </c>
-      <c r="B48" s="72"/>
-      <c r="C48" s="65" t="s">
-        <v>891</v>
-      </c>
-      <c r="D48" s="88" t="s">
-        <v>841</v>
-      </c>
-      <c r="E48" s="195" t="s">
-        <v>776</v>
-      </c>
-      <c r="F48" s="125" t="s">
+      <c r="A48" s="263">
+        <v>42736</v>
+      </c>
+      <c r="B48" s="430"/>
+      <c r="C48" s="73" t="s">
+        <v>882</v>
+      </c>
+      <c r="D48" s="265" t="s">
+        <v>392</v>
+      </c>
+      <c r="E48" s="429" t="s">
+        <v>943</v>
+      </c>
+      <c r="F48" s="266" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="263">
-        <v>42736</v>
-      </c>
-      <c r="B49" s="430"/>
-      <c r="C49" s="73" t="s">
+      <c r="A49" s="60">
+        <v>42736</v>
+      </c>
+      <c r="B49" s="81"/>
+      <c r="C49" s="62" t="s">
         <v>882</v>
       </c>
-      <c r="D49" s="265" t="s">
-        <v>392</v>
+      <c r="D49" s="65" t="s">
+        <v>941</v>
       </c>
       <c r="E49" s="429" t="s">
         <v>943</v>
       </c>
-      <c r="F49" s="266" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="60">
-        <v>42736</v>
-      </c>
-      <c r="B50" s="81"/>
-      <c r="C50" s="62" t="s">
-        <v>882</v>
-      </c>
-      <c r="D50" s="65" t="s">
-        <v>941</v>
-      </c>
-      <c r="E50" s="429" t="s">
-        <v>943</v>
-      </c>
-      <c r="F50" s="115" t="s">
+      <c r="F49" s="115" t="s">
         <v>339</v>
       </c>
     </row>

</xml_diff>